<commit_message>
Refactored folder structure, integrated Extent Report with screenshots, and added failure reason to Excel log
</commit_message>
<xml_diff>
--- a/src/test/resources/POC_data_sheet_v1.1.xlsx
+++ b/src/test/resources/POC_data_sheet_v1.1.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPidugujothi\IdeaProjects\AutomationPOC\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA8CFD-92B6-4452-9E07-F26F8EED1EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4B835D-18C1-4B92-AA7A-7B586C8F61A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{08B05D20-EDEF-43CA-A5DF-998FB408C439}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{08B05D20-EDEF-43CA-A5DF-998FB408C439}"/>
   </bookViews>
   <sheets>
     <sheet name="Common_TestData" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="131">
   <si>
     <t>Application</t>
   </si>
@@ -110,9 +110,6 @@
     <t>chennai</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Order ID</t>
   </si>
   <si>
@@ -321,12 +318,127 @@
   </si>
   <si>
     <t>Address 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latest Run ID </t>
+  </si>
+  <si>
+    <t>1969024</t>
+  </si>
+  <si>
+    <t>04/25/2025</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>15:03:56</t>
+  </si>
+  <si>
+    <t>1969245</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>17:49:39</t>
+  </si>
+  <si>
+    <t>1969279</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>18:10:09</t>
+  </si>
+  <si>
+    <t>1969285</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>18:15:19</t>
+  </si>
+  <si>
+    <t>1969332</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>19:10:46</t>
+  </si>
+  <si>
+    <t>1969350</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>19:25:24</t>
+  </si>
+  <si>
+    <t>1969378</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>20:02:30</t>
+  </si>
+  <si>
+    <t>1969383</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>20:07:17</t>
+  </si>
+  <si>
+    <t>1969390</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>20:22:04</t>
+  </si>
+  <si>
+    <t>Failure Reason</t>
+  </si>
+  <si>
+    <t>Execution Details</t>
+  </si>
+  <si>
+    <t>Application Output</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>21:10:25</t>
+  </si>
+  <si>
+    <t>org.openqa.selenium.NoSuchWindowException: no such window: target window already closed</t>
+  </si>
+  <si>
+    <t>1969433</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>21:10:55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,13 +503,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,43 +554,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -582,26 +657,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -654,42 +732,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1033,28 +1116,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="18" width="8.44140625"/>
+    <col min="2" max="2" customWidth="true" width="31.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5546875"/>
+    <col min="6" max="6" customWidth="true" width="20.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>30</v>
-      </c>
       <c r="C1" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>0</v>
@@ -1062,39 +1145,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -1113,50 +1196,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBDDBCF-8BF7-4A20-A442-6B433E5992DA}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="10"/>
-    <col min="3" max="3" width="13.5546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="40.21875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="12" style="10" customWidth="1"/>
-    <col min="9" max="9" width="29.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" style="10" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="10" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="10" customWidth="1"/>
-    <col min="18" max="18" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.77734375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="10"/>
-    <col min="21" max="21" width="21.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.21875" style="10" customWidth="1"/>
-    <col min="25" max="25" width="12.5546875" style="10" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="1" customWidth="true" style="10" width="16.44140625"/>
+    <col min="2" max="2" style="10" width="8.88671875"/>
+    <col min="3" max="3" customWidth="true" style="10" width="13.5546875"/>
+    <col min="4" max="4" customWidth="true" style="10" width="26.21875"/>
+    <col min="5" max="5" customWidth="true" style="10" width="40.21875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="7.44140625"/>
+    <col min="7" max="7" customWidth="true" style="10" width="10.6640625"/>
+    <col min="8" max="8" customWidth="true" style="10" width="12.0"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="10" width="29.21875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="10" width="11.5546875"/>
+    <col min="11" max="11" customWidth="true" style="10" width="15.109375"/>
+    <col min="12" max="12" customWidth="true" style="10" width="7.6640625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="10" width="15.77734375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="10" width="15.109375"/>
+    <col min="15" max="15" customWidth="true" style="10" width="20.0"/>
+    <col min="16" max="16" customWidth="true" style="10" width="7.6640625"/>
+    <col min="17" max="17" customWidth="true" style="10" width="12.77734375"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="10" width="11.0"/>
+    <col min="19" max="19" customWidth="true" style="10" width="12.77734375"/>
+    <col min="20" max="20" style="10" width="8.88671875"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="10" width="21.77734375"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="10" width="13.6640625"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="10" width="13.44140625"/>
+    <col min="24" max="24" customWidth="true" style="10" width="15.21875"/>
+    <col min="25" max="25" customWidth="true" style="10" width="12.5546875"/>
+    <col min="26" max="16384" style="10" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
@@ -1179,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>14</v>
@@ -1188,13 +1271,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>4</v>
@@ -1209,7 +1292,7 @@
         <v>7</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>12</v>
@@ -1229,31 +1312,31 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>18</v>
@@ -1268,10 +1351,10 @@
         <v>20</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>22</v>
@@ -1285,55 +1368,55 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="L4" s="6">
         <v>589556</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="O4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="R4" s="6">
         <v>8956545222</v>
@@ -1341,22 +1424,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>16</v>
@@ -1380,7 +1463,7 @@
         <v>20</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>21</v>
@@ -1413,43 +1496,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087D34EC-64B6-464A-B1FA-1B3B12C5A42D}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.77734375"/>
+    <col min="5" max="5" customWidth="true" width="36.5546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.77734375"/>
+    <col min="7" max="7" customWidth="true" width="14.5546875"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="10" max="10" customWidth="true" width="10.44140625"/>
+    <col min="11" max="11" customWidth="true" width="11.88671875"/>
+    <col min="12" max="12" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+    <row r="1" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="33"/>
       <c r="H1" s="33"/>
-      <c r="I1" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="35"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="35" t="s">
+        <v>124</v>
+      </c>
       <c r="K1" s="35"/>
     </row>
-    <row r="2" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1457,319 +1543,467 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="K4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="27"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="27" t="s">
+      <c r="F5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="J5" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="27"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="27"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="27"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" s="27"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="27"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="F15" t="s" s="36">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s" s="36">
+        <v>95</v>
+      </c>
+      <c r="H15" t="s" s="36">
+        <v>126</v>
+      </c>
+      <c r="I15" t="s" s="36">
+        <v>72</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" t="s" s="36">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s" s="38">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s" s="38">
+        <v>95</v>
+      </c>
+      <c r="H16" t="s" s="38">
+        <v>130</v>
+      </c>
+      <c r="I16" t="s" s="38">
+        <v>78</v>
+      </c>
+      <c r="J16" t="s" s="37">
+        <v>128</v>
+      </c>
+      <c r="K16" t="s" s="37">
+        <v>95</v>
+      </c>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1777,14 +2011,15 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1792,14 +2027,15 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="27"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="1"/>
@@ -1807,14 +2043,17 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
+      <c r="L20" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:K1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1823,25 +2062,25 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-    <col min="5" max="5" width="34.77734375" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="2" max="2" customWidth="true" width="16.77734375"/>
+    <col min="3" max="3" customWidth="true" width="15.77734375"/>
+    <col min="4" max="4" customWidth="true" width="27.109375"/>
+    <col min="5" max="5" customWidth="true" width="34.77734375"/>
+    <col min="6" max="6" customWidth="true" width="13.5546875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.44140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.6640625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.88671875"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.6640625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1849,51 +2088,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>55</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1903,22 +2142,22 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1928,22 +2167,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>

</xml_diff>

<commit_message>
feat: Automation POC framework enhancements
- Implemented email sending feature with report attachment after test execution.
- Integrated ExtentReports dynamic generation and HTML report saving.
- Improved SMTP password handling with encryption and environment variable fallback for security.
- General framework polishing and structure improvements.
</commit_message>
<xml_diff>
--- a/src/test/resources/POC_data_sheet_v1.1.xlsx
+++ b/src/test/resources/POC_data_sheet_v1.1.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPidugujothi\IdeaProjects\AutomationPOC\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4B835D-18C1-4B92-AA7A-7B586C8F61A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B713EB0D-BD09-460D-BF11-31F9B9488895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{08B05D20-EDEF-43CA-A5DF-998FB408C439}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="184">
   <si>
     <t>Application</t>
   </si>
@@ -432,13 +432,171 @@
   </si>
   <si>
     <t>21:10:55</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>04/27/2025</t>
+  </si>
+  <si>
+    <t>14:17:57</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[@class='sub-category-...</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>15:05:58</t>
+  </si>
+  <si>
+    <t>Login was not successful for user: testUser@myridius.com</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>15:20:13</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to be clickable: Proxy element for: DefaultElementLoc...</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>15:26:23</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of [[ChromeDriver: chrome on windows (578491c299e1...</t>
+  </si>
+  <si>
+    <t>1970038</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>15:28:43</t>
+  </si>
+  <si>
+    <t>1970057</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>15:54:15</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>18:33:48</t>
+  </si>
+  <si>
+    <t>io.github.bonigarcia.wdm.config.WebDriverManagerException: java.net.UnknownHostException: googlechro...</t>
+  </si>
+  <si>
+    <t>1970456</t>
+  </si>
+  <si>
+    <t>04/28/2025</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>10:20:58</t>
+  </si>
+  <si>
+    <t>1970461</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>10:32:51</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>10:36:31</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on windows (b...</t>
+  </si>
+  <si>
+    <t>1970480</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>11:00:23</t>
+  </si>
+  <si>
+    <t>1970514</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>11:30:27</t>
+  </si>
+  <si>
+    <t>1970528</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>11:52:46</t>
+  </si>
+  <si>
+    <t>1970560</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>12:21:34</t>
+  </si>
+  <si>
+    <t>1970586</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>12:49:19</t>
+  </si>
+  <si>
+    <t>1970623</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>13:31:32</t>
+  </si>
+  <si>
+    <t>1970630</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>13:46:42</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,7 +672,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -572,17 +730,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -596,90 +743,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,7 +760,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -732,20 +800,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,24 +816,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1116,70 +1178,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="18" width="8.44140625"/>
-    <col min="2" max="2" customWidth="true" width="31.44140625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5546875"/>
-    <col min="6" max="6" customWidth="true" width="20.109375"/>
+    <col min="1" max="1" width="8.44140625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1202,279 +1264,279 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="10" width="16.44140625"/>
-    <col min="2" max="2" style="10" width="8.88671875"/>
-    <col min="3" max="3" customWidth="true" style="10" width="13.5546875"/>
-    <col min="4" max="4" customWidth="true" style="10" width="26.21875"/>
-    <col min="5" max="5" customWidth="true" style="10" width="40.21875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="7.44140625"/>
-    <col min="7" max="7" customWidth="true" style="10" width="10.6640625"/>
-    <col min="8" max="8" customWidth="true" style="10" width="12.0"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="10" width="29.21875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="10" width="11.5546875"/>
-    <col min="11" max="11" customWidth="true" style="10" width="15.109375"/>
-    <col min="12" max="12" customWidth="true" style="10" width="7.6640625"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="10" width="15.77734375"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="10" width="15.109375"/>
-    <col min="15" max="15" customWidth="true" style="10" width="20.0"/>
-    <col min="16" max="16" customWidth="true" style="10" width="7.6640625"/>
-    <col min="17" max="17" customWidth="true" style="10" width="12.77734375"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="10" width="11.0"/>
-    <col min="19" max="19" customWidth="true" style="10" width="12.77734375"/>
-    <col min="20" max="20" style="10" width="8.88671875"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="10" width="21.77734375"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="10" width="13.6640625"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="10" width="13.44140625"/>
-    <col min="24" max="24" customWidth="true" style="10" width="15.21875"/>
-    <col min="25" max="25" customWidth="true" style="10" width="12.5546875"/>
-    <col min="26" max="16384" style="10" width="8.88671875"/>
+    <col min="1" max="1" width="16.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="9"/>
+    <col min="3" max="3" width="13.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="40.21875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="12" style="9" customWidth="1"/>
+    <col min="9" max="9" width="29.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="9" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="9" customWidth="1"/>
+    <col min="18" max="18" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.77734375" style="9" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="9"/>
+    <col min="21" max="21" width="21.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.21875" style="9" customWidth="1"/>
+    <col min="25" max="25" width="12.5546875" style="9" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="30"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>456789</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>2536588589</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>589556</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>8956545222</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>456789</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>2536588589</v>
       </c>
     </row>
@@ -1496,554 +1558,1223 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087D34EC-64B6-464A-B1FA-1B3B12C5A42D}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.88671875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.77734375"/>
-    <col min="5" max="5" customWidth="true" width="36.5546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.77734375"/>
-    <col min="7" max="7" customWidth="true" width="14.5546875"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="14.88671875"/>
-    <col min="10" max="10" customWidth="true" width="10.44140625"/>
-    <col min="11" max="11" customWidth="true" width="11.88671875"/>
-    <col min="12" max="12" customWidth="true" width="15.0"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="32" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="35" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:12" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="28" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="27"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="27"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="27"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="27" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="27"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="20"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="20"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="20"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="20"/>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="20"/>
+    </row>
+    <row r="17" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L22" s="20"/>
+    </row>
+    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L24" s="20"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L27" s="20"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L28" s="20"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L29" s="20"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L30" s="20"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L32" s="20"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L33" s="20"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="27"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="5" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" s="27"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F15" t="s" s="36">
-        <v>125</v>
-      </c>
-      <c r="G15" t="s" s="36">
-        <v>95</v>
-      </c>
-      <c r="H15" t="s" s="36">
-        <v>126</v>
-      </c>
-      <c r="I15" t="s" s="36">
-        <v>72</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" t="s" s="36">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="5" t="s">
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F16" t="s" s="38">
-        <v>129</v>
-      </c>
-      <c r="G16" t="s" s="38">
-        <v>95</v>
-      </c>
-      <c r="H16" t="s" s="38">
-        <v>130</v>
-      </c>
-      <c r="I16" t="s" s="38">
-        <v>78</v>
-      </c>
-      <c r="J16" t="s" s="37">
-        <v>128</v>
-      </c>
-      <c r="K16" t="s" s="37">
-        <v>95</v>
-      </c>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="27"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="27"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="5" t="s">
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="27"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2067,17 +2798,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.44140625"/>
-    <col min="2" max="2" customWidth="true" width="16.77734375"/>
-    <col min="3" max="3" customWidth="true" width="15.77734375"/>
-    <col min="4" max="4" customWidth="true" width="27.109375"/>
-    <col min="5" max="5" customWidth="true" width="34.77734375"/>
-    <col min="6" max="6" customWidth="true" width="13.5546875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.44140625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.6640625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.88671875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.6640625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.77734375"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="34.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2096,7 +2827,7 @@
       <c r="E1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="19" t="s">
         <v>93</v>
       </c>
       <c r="G1" s="2" t="s">

</xml_diff>